<commit_message>
function to add calory values to calory table
</commit_message>
<xml_diff>
--- a/Muscle Macros.xlsx
+++ b/Muscle Macros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a2031a7135c679e/Exercises/fitness/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{96FC399A-D58B-448F-9524-59E95A71F716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9F82573-009B-47E9-8347-790C503184CF}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{96FC399A-D58B-448F-9524-59E95A71F716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68EE1E90-C13D-4E04-A70D-6335BB803637}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{2911207B-D3EF-4C79-89D7-50B62DA5792A}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="72">
   <si>
     <t>Meals</t>
   </si>
@@ -2254,7 +2254,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F51E392-74CE-46D4-9E2A-8FBF7769E028}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="G1:J1"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:J1"/>
@@ -2276,6 +2276,11 @@
         <v>70</v>
       </c>
     </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>